<commit_message>
chore : update work log
</commit_message>
<xml_diff>
--- a/Journal-de-Travail_SanchezFilipeEithan.xlsx
+++ b/Journal-de-Travail_SanchezFilipeEithan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pa78gum\Documents\GitHub\PassionLectureMobile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5A9974-AE7A-4949-91E0-5F5346D2D7BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE825FE-4584-483E-9538-05AC3921598E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">'Journal de travail'!$A$6:$G$6</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,6 +32,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -136,6 +137,9 @@
   </si>
   <si>
     <t>Réalisation de la maquette de la d'un livre</t>
+  </si>
+  <si>
+    <t>Création du projet de base</t>
   </si>
 </sst>
 </file>
@@ -1066,7 +1070,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1.0416666666666666E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1081,7 +1085,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.4305555555555556E-2</c:v>
+                  <c:v>4.8611111111111112E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1997,7 +2001,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2050,7 +2054,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 0 heurs 50 minutes</v>
+        <v>0 jours 1 heurs 25 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2069,11 +2073,11 @@
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2117,7 +2121,7 @@
       </c>
       <c r="C7" s="43"/>
       <c r="D7" s="44">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E7" s="45" t="s">
         <v>21</v>
@@ -2137,7 +2141,7 @@
       </c>
       <c r="C8" s="47"/>
       <c r="D8" s="48">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E8" s="49" t="s">
         <v>21</v>
@@ -2166,9 +2170,11 @@
       </c>
       <c r="C9" s="51"/>
       <c r="D9" s="52">
-        <v>15</v>
-      </c>
-      <c r="E9" s="53"/>
+        <v>20</v>
+      </c>
+      <c r="E9" s="53" t="s">
+        <v>21</v>
+      </c>
       <c r="F9" s="36" t="s">
         <v>30</v>
       </c>
@@ -2184,15 +2190,23 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="str">
+      <c r="A10" s="8">
         <f>IF(ISBLANK(B10),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B10))</f>
-        <v/>
-      </c>
-      <c r="B10" s="46"/>
+        <v>13</v>
+      </c>
+      <c r="B10" s="46">
+        <v>45740</v>
+      </c>
       <c r="C10" s="47"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="36"/>
+      <c r="D10" s="48">
+        <v>15</v>
+      </c>
+      <c r="E10" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="36" t="s">
+        <v>32</v>
+      </c>
       <c r="G10" s="55"/>
       <c r="M10" t="s">
         <v>5</v>
@@ -8631,7 +8645,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8639,7 +8653,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0</v>
+        <v>1.0416666666666666E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8721,7 +8735,7 @@
       </c>
       <c r="B10">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C10,'Journal de travail'!$D$7:$D$532)</f>
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="C10" s="37" t="str">
         <f>'Journal de travail'!M14</f>
@@ -8729,7 +8743,7 @@
       </c>
       <c r="D10" s="33">
         <f t="shared" si="0"/>
-        <v>2.4305555555555556E-2</v>
+        <v>4.8611111111111112E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -8756,7 +8770,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>2.4305555555555556E-2</v>
+        <v>5.9027777777777776E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8781,15 +8795,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9012,6 +9017,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
@@ -9024,14 +9038,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9048,4 +9054,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat : add detail page (with title and cover)
</commit_message>
<xml_diff>
--- a/Journal-de-Travail_SanchezFilipeEithan.xlsx
+++ b/Journal-de-Travail_SanchezFilipeEithan.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pa78gum\Documents\GitHub\PassionLectureMobile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8730B1F2-4246-49D3-AAB5-A2C59CB06B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD2BD04-DF2B-4E28-9C7B-D272B65395ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -157,7 +157,19 @@
     <t>Savoir qu'est ce qu'un epub et comment le gérer avec node.js</t>
   </si>
   <si>
-    <t>Renvoie la cover</t>
+    <t>Renvoie un objet  avec l'id du livre, titre et image</t>
+  </si>
+  <si>
+    <t>Renvoie la cover (WIP)</t>
+  </si>
+  <si>
+    <t>Recherche sur comment renvoyer une image</t>
+  </si>
+  <si>
+    <t>Renvoie tous les livres disponibles avec l'image en base64</t>
+  </si>
+  <si>
+    <t>Appel l'api recoupere tout les livres puis les affiche</t>
   </si>
 </sst>
 </file>
@@ -341,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -477,11 +489,88 @@
     <xf numFmtId="20" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -651,80 +740,6 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1088,13 +1103,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.11458333333333333</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.4722222222222224E-2</c:v>
+                  <c:v>4.5138888888888888E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1812,18 +1827,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
   <autoFilter ref="A6:G532" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="14">
       <calculatedColumnFormula>IF(ISBLANK(B7),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="heure" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Activité" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarque / problème" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="heure" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Activité" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarque / problème" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2019,7 +2034,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2072,7 +2087,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 5 heurs 4 minutes</v>
+        <v>0 jours 8 heurs 35 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2087,15 +2102,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>185</v>
+        <v>275</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>305</v>
+        <v>515</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2401,7 +2416,7 @@
         <v>4</v>
       </c>
       <c r="F16" s="36" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G16" s="55"/>
       <c r="O16">
@@ -2409,60 +2424,96 @@
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="str">
+      <c r="A17" s="16">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B17))</f>
-        <v/>
-      </c>
-      <c r="B17" s="50"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="36"/>
+        <v>18</v>
+      </c>
+      <c r="B17" s="50">
+        <v>45775</v>
+      </c>
+      <c r="C17" s="51">
+        <v>1</v>
+      </c>
+      <c r="D17" s="52">
+        <v>30</v>
+      </c>
+      <c r="E17" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="36" t="s">
+        <v>38</v>
+      </c>
       <c r="G17" s="56"/>
       <c r="O17">
         <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="str">
+      <c r="A18" s="8">
         <f>IF(ISBLANK(B18),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B18))</f>
-        <v/>
-      </c>
-      <c r="B18" s="46"/>
+        <v>18</v>
+      </c>
+      <c r="B18" s="46">
+        <v>45775</v>
+      </c>
       <c r="C18" s="47"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="36"/>
+      <c r="D18" s="48">
+        <v>15</v>
+      </c>
+      <c r="E18" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="36" t="s">
+        <v>40</v>
+      </c>
       <c r="G18" s="55"/>
       <c r="O18">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="str">
+      <c r="A19" s="16">
         <f>IF(ISBLANK(B19),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B19))</f>
-        <v/>
-      </c>
-      <c r="B19" s="50"/>
-      <c r="C19" s="51"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="36"/>
+        <v>19</v>
+      </c>
+      <c r="B19" s="50">
+        <v>45782</v>
+      </c>
+      <c r="C19" s="47"/>
+      <c r="D19" s="52">
+        <v>30</v>
+      </c>
+      <c r="E19" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="36" t="s">
+        <v>41</v>
+      </c>
       <c r="G19" s="56"/>
       <c r="O19">
         <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="str">
+      <c r="A20" s="8">
         <f>IF(ISBLANK(B20),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B20))</f>
-        <v/>
-      </c>
-      <c r="B20" s="46"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="36"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="46">
+        <v>45782</v>
+      </c>
+      <c r="C20" s="59">
+        <v>1</v>
+      </c>
+      <c r="D20" s="48">
+        <v>15</v>
+      </c>
+      <c r="E20" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="36" t="s">
+        <v>42</v>
+      </c>
       <c r="G20" s="55"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -8616,40 +8667,40 @@
     <mergeCell ref="C5:D5"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:E532">
-    <cfRule type="expression" dxfId="16" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>$E7="Autre"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
       <formula>$E7="Design"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
       <formula>$E7="Présentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
       <formula>$E7="Meeting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
       <formula>$E7="Documentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="6" stopIfTrue="1">
       <formula>$E7="Test"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="7" stopIfTrue="1">
       <formula>$E7="Analyse"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="9" stopIfTrue="1">
       <formula>$E7="Développement"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:C532" xr:uid="{9D52E29F-610D-40B2-B3CC-F94A741DD978}">
-      <formula1>$N$7:$N$15</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D532" xr:uid="{46510F84-8BCC-4BD6-9A19-9F03ACD74D05}">
       <formula1>$O$7:$O$19</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E532" xr:uid="{5717AF9A-5C26-4256-9473-8948342ED6D3}">
       <formula1>$M$7:$M$15</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C21:C532 C7:C19" xr:uid="{9D52E29F-610D-40B2-B3CC-F94A741DD978}">
+      <formula1>$N$7:$N$15</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8711,11 +8762,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>45</v>
+        <v>120</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8723,7 +8774,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.11458333333333333</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8751,7 +8802,7 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="C7" s="27" t="str">
         <f>'Journal de travail'!M11</f>
@@ -8759,7 +8810,7 @@
       </c>
       <c r="D7" s="33">
         <f t="shared" si="0"/>
-        <v>3.4722222222222224E-2</v>
+        <v>4.5138888888888888E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -8840,7 +8891,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.21180555555555555</v>
+        <v>0.3576388888888889</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8865,15 +8916,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9096,6 +9138,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
@@ -9108,14 +9159,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9132,4 +9175,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat : adapt back en to send chapters too
</commit_message>
<xml_diff>
--- a/Journal-de-Travail_SanchezFilipeEithan.xlsx
+++ b/Journal-de-Travail_SanchezFilipeEithan.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pa78gum\Documents\GitHub\PassionLectureMobile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD2BD04-DF2B-4E28-9C7B-D272B65395ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0ABD94-E71F-4E01-8CCC-A87AA5F7D6F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -170,6 +170,12 @@
   </si>
   <si>
     <t>Appel l'api recoupere tout les livres puis les affiche</t>
+  </si>
+  <si>
+    <t>Page de livre detaillé</t>
+  </si>
+  <si>
+    <t>Récuperer les chapitres dans le backend</t>
   </si>
 </sst>
 </file>
@@ -482,6 +488,9 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -489,88 +498,11 @@
     <xf numFmtId="20" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -740,6 +672,80 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1103,7 +1109,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25</c:v>
+                  <c:v>0.31944444444444442</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1827,18 +1833,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
   <autoFilter ref="A6:G532" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="14">
+    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="6">
       <calculatedColumnFormula>IF(ISBLANK(B7),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="heure" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Activité" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarque / problème" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="heure" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Activité" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarque / problème" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2033,8 +2039,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
+      <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2069,11 +2075,11 @@
       <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
       <c r="F2" s="5" t="s">
         <v>2</v>
       </c>
@@ -2087,7 +2093,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 8 heurs 35 minutes</v>
+        <v>0 jours 10 heurs 15 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2102,24 +2108,24 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>240</v>
+        <v>300</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>275</v>
+        <v>315</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>515</v>
+        <v>615</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="58" t="s">
+      <c r="C5" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="58"/>
+      <c r="D5" s="59"/>
     </row>
     <row r="6" spans="1:15" s="20" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
@@ -2502,7 +2508,7 @@
       <c r="B20" s="46">
         <v>45782</v>
       </c>
-      <c r="C20" s="59">
+      <c r="C20" s="57">
         <v>1</v>
       </c>
       <c r="D20" s="48">
@@ -2517,27 +2523,45 @@
       <c r="G20" s="55"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="str">
+      <c r="A21" s="16">
         <f>IF(ISBLANK(B21),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B21))</f>
-        <v/>
-      </c>
-      <c r="B21" s="50"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="36"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="50">
+        <v>45789</v>
+      </c>
+      <c r="C21" s="51">
+        <v>1</v>
+      </c>
+      <c r="D21" s="52">
+        <v>10</v>
+      </c>
+      <c r="E21" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="36" t="s">
+        <v>43</v>
+      </c>
       <c r="G21" s="56"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="str">
+      <c r="A22" s="8">
         <f>IF(ISBLANK(B22),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B22))</f>
-        <v/>
-      </c>
-      <c r="B22" s="46"/>
+        <v>20</v>
+      </c>
+      <c r="B22" s="46">
+        <v>45789</v>
+      </c>
       <c r="C22" s="47"/>
-      <c r="D22" s="48"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="36"/>
+      <c r="D22" s="48">
+        <v>30</v>
+      </c>
+      <c r="E22" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="36" t="s">
+        <v>44</v>
+      </c>
       <c r="G22" s="55"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -8667,28 +8691,28 @@
     <mergeCell ref="C5:D5"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:E532">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="16" priority="1">
       <formula>$E7="Autre"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="2" stopIfTrue="1">
       <formula>$E7="Design"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="3" stopIfTrue="1">
       <formula>$E7="Présentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="4" stopIfTrue="1">
       <formula>$E7="Meeting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="5" stopIfTrue="1">
       <formula>$E7="Documentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="6" stopIfTrue="1">
       <formula>$E7="Test"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="7" stopIfTrue="1">
       <formula>$E7="Analyse"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
       <formula>$E7="Développement"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8762,11 +8786,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>240</v>
+        <v>300</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8774,7 +8798,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.25</v>
+        <v>0.31944444444444442</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8891,7 +8915,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.3576388888888889</v>
+        <v>0.42708333333333331</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8916,6 +8940,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9138,15 +9171,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
@@ -9159,6 +9183,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9175,12 +9207,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>